<commit_message>
Commit the whole directroy
</commit_message>
<xml_diff>
--- a/src/test/java/com/Test_Data/Emp_Data.xlsx
+++ b/src/test/java/com/Test_Data/Emp_Data.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="21425"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Automation_Practise\src\test\java\com\Test_Data\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E6BEF7DF-7E0C-426F-9E44-285B1F12E8FC}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="60" windowWidth="20115" windowHeight="8010"/>
+    <workbookView xWindow="-96" yWindow="-96" windowWidth="19392" windowHeight="10392" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,9 +42,6 @@
     <t>Delta</t>
   </si>
   <si>
-    <t>Freddie</t>
-  </si>
-  <si>
     <t>Email_ID</t>
   </si>
   <si>
@@ -54,28 +57,31 @@
     <t>delta@live.com</t>
   </si>
   <si>
-    <t>freddie@msn.com</t>
-  </si>
-  <si>
     <t>A01</t>
   </si>
   <si>
-    <t>A02</t>
-  </si>
-  <si>
-    <t>A03</t>
-  </si>
-  <si>
-    <t>A04</t>
-  </si>
-  <si>
-    <t>A05</t>
+    <t>B02</t>
+  </si>
+  <si>
+    <t>C03</t>
+  </si>
+  <si>
+    <t>D04</t>
+  </si>
+  <si>
+    <t>E05</t>
+  </si>
+  <si>
+    <t>echo@msn.com</t>
+  </si>
+  <si>
+    <t>Echo</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -136,6 +142,9 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
   </extLst>
 </styleSheet>
 </file>
@@ -183,7 +192,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -216,9 +225,26 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -251,6 +277,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -426,23 +469,23 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12:C13"/>
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
-    <col min="1" max="1" width="9.140625" style="1"/>
-    <col min="2" max="2" width="13.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="19.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="35.85546875" style="1" customWidth="1"/>
-    <col min="5" max="6" width="9.140625" style="1"/>
+    <col min="1" max="1" width="9.15625" style="1"/>
+    <col min="2" max="2" width="13.26171875" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="19.15625" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="35.83984375" style="1" customWidth="1"/>
+    <col min="5" max="6" width="9.15625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -450,95 +493,95 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" s="1" t="s">
         <v>3</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" s="1" t="s">
         <v>4</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" s="1" t="s">
         <v>5</v>
       </c>
       <c r="B5" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A6" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C6" s="3" t="s">
         <v>16</v>
-      </c>
-      <c r="C5" s="3" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="C6" s="3" t="s">
-        <v>12</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="C2" r:id="rId1"/>
-    <hyperlink ref="C3" r:id="rId2"/>
-    <hyperlink ref="C4" r:id="rId3"/>
-    <hyperlink ref="C5" r:id="rId4"/>
-    <hyperlink ref="C6" r:id="rId5"/>
+    <hyperlink ref="C2" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="C3" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
+    <hyperlink ref="C4" r:id="rId3" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
+    <hyperlink ref="C5" r:id="rId4" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
+    <hyperlink ref="C6" r:id="rId5" xr:uid="{00000000-0004-0000-0000-000004000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>